<commit_message>
Added R2M2E2 files, updated README
</commit_message>
<xml_diff>
--- a/DM1092_ESP32_Embedded_WIFI_BT_IMU/Docs/Assembly Outputs/BOM/BOM-DM1092_ACTIVE_BOM(Production).xlsx
+++ b/DM1092_ESP32_Embedded_WIFI_BT_IMU/Docs/Assembly Outputs/BOM/BOM-DM1092_ACTIVE_BOM(Production).xlsx
@@ -306,7 +306,7 @@
     <t>A12N02A-201_1.6mmbrd_MatedModule</t>
   </si>
   <si>
-    <t>A12N02A-201_Connector_(1.6mm_brd)</t>
+    <t>A12N02A-201_Connector</t>
   </si>
   <si>
     <t>BBR43-24KB533 for camera module TG161B-201</t>
@@ -390,7 +390,7 @@
     <t>105450-0101</t>
   </si>
   <si>
-    <t>QWIIC, side entry</t>
+    <t>QUIIC, side entry</t>
   </si>
   <si>
     <t>J11</t>
@@ -823,21 +823,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,9 +1130,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1158,1588 +1146,1569 @@
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>9</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>4</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="1">
         <v>3</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="1">
         <v>18</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="1">
         <v>3</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="1">
         <v>6</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="2" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="1">
         <v>2</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I42" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B47" s="4">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="I48" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="I49" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="I50" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="1">
         <v>2</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="I51" s="3" t="s">
+      <c r="I51" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="I52" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B53" s="4">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="2" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="29" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>